<commit_message>
Python sql assignment 2
</commit_message>
<xml_diff>
--- a/query/query1.xlsx
+++ b/query/query1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>7902</t>
+          <t>FORD</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>7698</t>
+          <t>BLAKE</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7698</t>
+          <t>BLAKE</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>7839</t>
+          <t>KING</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>7698</t>
+          <t>BLAKE</t>
         </is>
       </c>
     </row>
@@ -548,7 +548,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>7839</t>
+          <t>KING</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>7839</t>
+          <t>KING</t>
         </is>
       </c>
     </row>
@@ -582,105 +582,92 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>7566</t>
+          <t>JONES</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>7839</t>
+          <t>7844</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>KING</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
+          <t>TURNER</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>BLAKE</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>7844</t>
+          <t>7876</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>TURNER</t>
+          <t>ADAMS</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>7698</t>
+          <t>SCOTT</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>7876</t>
+          <t>7900</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ADAMS</t>
+          <t>JAMES</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>7788</t>
+          <t>BLAKE</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>7900</t>
+          <t>7902</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>JAMES</t>
+          <t>FORD</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7698</t>
+          <t>JONES</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>7902</t>
+          <t>7934</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>FORD</t>
+          <t>MILLER</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>7566</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>7934</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>MILLER</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>7782</t>
+          <t>CLARK</t>
         </is>
       </c>
     </row>

</xml_diff>